<commit_message>
Inventory automation and some javadoc
</commit_message>
<xml_diff>
--- a/restaurantmanager/src/main/resources/Ingredients.xlsx
+++ b/restaurantmanager/src/main/resources/Ingredients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Cpsc - 488\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Cpsc - 488\Git\MasterRepo\Fall-2022---Group-7---Restaurant-Management-Assisstant\restaurantmanager\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{967E49AC-A957-4355-A11B-0323FCBA558B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652CA954-FDC0-4C02-9BF3-32C2D94E1CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{02319B65-2503-47F0-99F1-E9F798E29077}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02319B65-2503-47F0-99F1-E9F798E29077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>chicken nuggets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot dog </t>
   </si>
 </sst>
 </file>
@@ -420,13 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5394468F-A14F-4B41-9EF9-5FA38C4D8BA2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -524,6 +530,17 @@
         <v>10</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
         <v>0</v>
       </c>
     </row>

</xml_diff>